<commit_message>
beta 1 version camera ready
</commit_message>
<xml_diff>
--- a/imagenesPrueba/100_IM-0002-1001/resultados.xlsx
+++ b/imagenesPrueba/100_IM-0002-1001/resultados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20055" windowHeight="6405"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="resultados" sheetId="1" r:id="rId1"/>
@@ -597,6 +597,7 @@
   <c:lang val="es-ES"/>
   <c:style val="1"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -2469,2479 +2470,34 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>resultados!$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>dominadas</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>resultados!$E$303:$E$704</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="402"/>
-                <c:pt idx="0">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99803173402207124</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99817203587729875</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.98920999832865253</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.99575857355962127</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.86744520399608505</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.99754387505662623</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9040968132331888</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.95437079306445627</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.99806210851436505</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.95900850401133997</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.99814032313568124</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.8721993205822588</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.90457332714192995</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.92692286223937503</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.99788487904600498</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.99747345842064505</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.91660319498207998</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.99764554931418248</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.94195838944039378</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.99822034929577375</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.99815983707172629</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.98679723368285877</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.98922742760191873</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.93908527338169123</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.99821594161189875</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.93350658426898503</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.99793867250034629</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.88770983987411001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.94758280598132372</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.93295870779737877</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.94573294566198629</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.91126154303016249</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.98890072400933748</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.99737146774304497</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.88592115751250622</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.98593179913410001</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.85867632042974995</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.9936153296703375</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.91422223133277625</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.90457332714192995</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.86814907039728628</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.86499196667097999</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.99597845432683874</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.99816409426986497</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.98916699222599502</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.93241284959095749</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.99540742510786495</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.9380204156240538</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.94757743144396123</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.99754387505662623</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.96613105263918375</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.99814268281720253</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.95095686088313747</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.94479071635716005</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.90457332714192995</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.96758642238742376</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.99651664923768746</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.98919190889089004</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.86250331794838753</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.98590942734239995</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.87884452321568873</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.99668296932150746</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.9981036045752838</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.963554516494185</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.9399259928843513</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.9977366459685475</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.94592620779482628</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.88985322234824249</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.93966450829006498</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.99788487904600498</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.87105217993347628</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.94090287916106874</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.93768492102469625</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.9890964150262338</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.98885542636928003</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.99821245339918752</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.97632476236743249</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.99806371166854624</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.92481248136194749</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.88877147754225627</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.86955719009907628</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.98661983458258629</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.94548718497446627</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.99764554931418248</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.99806210851436505</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.9056416587636763</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.99821714473571999</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>0.90457332714192995</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>0.99653297108368</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0.99747345842064505</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.99737146774304497</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0.98914048556405376</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.98905473256954379</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>0.96766203321994371</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>0.96058656376610996</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.85603106305691246</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.99797210525032121</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>0.93743014233059996</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>0.86289117911389379</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.91527546919379876</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>0.99747345842064505</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>0.98898998041606878</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.95764383271888998</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>0.99814084266648995</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>0.99288687564060496</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.99791223866408874</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.8852583556071475</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>0.95601298440160376</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>0.92801072783873995</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>0.92045492574999621</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.99762132620825372</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0.88004570343423871</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>0.9981592212960787</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>0.99764554931418248</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>0.9977366459685475</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>0.94660379252217997</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>0.98941945609109505</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>0.95863016985959371</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>0.93071134822344004</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>0.9977366459685475</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>0.9978119620340612</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>0.90457332714192995</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>0.93069613953198371</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>0.89306245944506879</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>0.98892186290241879</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>0.86499196667097999</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>0.9977366459685475</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>0.99747345842064505</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>0.9440932858069212</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>0.85681153463897375</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>0.93251628877336878</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>0.96282783747625622</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>0.92691949961752251</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>0.92353577281395249</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>0.99815936712190378</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>0.99775286846019495</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>0.99811950263704496</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>0.88910793735694249</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>0.98918446592780751</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>0.93951118043860371</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>0.94861157552259745</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>0.87947389026128753</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>0.92288383258062001</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>0.86011842614678247</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>0.9111626325448513</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>0.96392875703081249</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>0.99764179134774622</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>0.90078193933160877</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>0.98947587349521127</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>0.86726183222900755</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>0.94358242183367247</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>0.93114058255845877</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>0.88476275266017246</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>0.98922742760191873</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>0.96331283246236121</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>0.91175913267706254</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>0.94889656366414499</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>0.9977366459685475</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>0.99747040877262005</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>0.85829627441332623</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>0.95993434075549755</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>0.99788487904600498</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>0.99764179134774622</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>0.99787908518236879</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>0.99810031179826375</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>0.9889951891912262</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>0.99817221364324626</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>0.94525522122494499</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>0.89363143196494121</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>0.8599494692865175</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>0.99747345842064505</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>0.95148376319612005</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>0.96316612797087753</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>0.88579556517999747</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>0.94051444346117752</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>0.99764179134774622</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>0.99811384134961623</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>0.99816532351864251</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>0.9979405009211012</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>0.98941945609109505</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>0.99817418973824501</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>0.88023542843325497</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>0.88271441160673747</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>0.99764554931418248</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>0.99797210525032121</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>0.94604558593759003</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>0.99806210851436505</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>0.99788487904600498</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>0.93660135688520252</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>0.99810031179826375</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>0.95070345508582499</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>0.99814441288015754</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>0.99764554931418248</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>0.86971550235491502</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>0.99788487904600498</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>0.92481248136194749</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>0.88595529060990252</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>0.89440546844896629</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>0.920182755826495</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>0.99636927185243995</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>0.9977186160138225</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>0.90851404242500877</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>0.93395029995749879</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>0.960895825734005</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>0.99681138533549374</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>0.99814088494782749</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>0.89561393655179622</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>0.99815615151250003</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>0.85601257209202497</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>0.93394623137909372</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>0.92612290932555752</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>0.9111932220838137</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>0.9923647744875137</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>0.86278823763553125</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>0.90457332714192995</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>0.98944398632921504</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>0.93260280869929624</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>0.86499196667097999</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>0.98908991806052371</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>0.9549939296309975</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>0.92409778328020253</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>0.90412036511060123</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>0.98939190336935623</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>0.99815729634960626</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>0.89209132784111878</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>0.93251628877336878</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>0.88402267716162253</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>0.90966741748409752</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>0.99814084266648995</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>0.9440932858069212</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>0.99812142643787127</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>0.99737146774304497</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>0.99747345842064505</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>0.98885120622881628</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>0.90219241787993998</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>0.99810955766549503</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>0.88221628717127121</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>0.90822128405739</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>0.99789098700851619</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>0.96802999201716255</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>0.94232041987579995</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>0.99429785868220999</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>0.99787630046676001</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>0.99812320940541122</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>0.88251511737490751</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>0.91694600633616752</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>0.93249258130341373</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>0.90030666489867872</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>0.88631108677648496</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>0.91826457682760121</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>0.98889490547727998</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>0.99764554931418248</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>0.99788487904600498</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>0.90966741748409752</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>0.9363098736370512</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>0.92144392091943128</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>0.86478051817426249</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>0.99819330819075625</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>0.99706677874959249</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>0.99787041505951624</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>0.9249261175382063</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>0.88004570343423871</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>0.88482015319883378</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>0.99785667168482128</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>0.91633189564319628</c:v>
-                </c:pt>
-                <c:pt idx="387">
-                  <c:v>0.9980954657230362</c:v>
-                </c:pt>
-                <c:pt idx="388">
-                  <c:v>0.90529368427276746</c:v>
-                </c:pt>
-                <c:pt idx="389">
-                  <c:v>0.91354558533698371</c:v>
-                </c:pt>
-                <c:pt idx="390">
-                  <c:v>0.99808828849060505</c:v>
-                </c:pt>
-                <c:pt idx="391">
-                  <c:v>0.8638734498268188</c:v>
-                </c:pt>
-                <c:pt idx="392">
-                  <c:v>0.98893969631930123</c:v>
-                </c:pt>
-                <c:pt idx="393">
-                  <c:v>0.89659727548154122</c:v>
-                </c:pt>
-                <c:pt idx="394">
-                  <c:v>0.9981819053934613</c:v>
-                </c:pt>
-                <c:pt idx="395">
-                  <c:v>0.96155589348514625</c:v>
-                </c:pt>
-                <c:pt idx="396">
-                  <c:v>0.86814907039728628</c:v>
-                </c:pt>
-                <c:pt idx="397">
-                  <c:v>0.85601257209202497</c:v>
-                </c:pt>
-                <c:pt idx="398">
-                  <c:v>0.93768492102469625</c:v>
-                </c:pt>
-                <c:pt idx="399">
-                  <c:v>0.98150266075899872</c:v>
-                </c:pt>
-                <c:pt idx="400">
-                  <c:v>0.99237058923529253</c:v>
-                </c:pt>
-                <c:pt idx="401">
-                  <c:v>0.99704104286613626</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>resultados!$I$303:$I$704</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="402"/>
-                <c:pt idx="0">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.51385756404072602</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.50432424948615195</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.74522131923253498</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.59619799325300804</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.96886519195201504</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.53137634041209103</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.94450401626749103</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.81992567992503096</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.513238468895725</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.81236460736642302</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.50452508501461801</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.98603389174234002</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.94718558089696803</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.84614643055524297</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.52091944970511395</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.53959584627359403</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.89712685358799305</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.53733983147650999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.79728383418183701</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.50858878331969903</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.50879700925877502</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.75069129220376296</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.74564630731308301</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.83737032236919395</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.50662762350212198</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.84518319270074604</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.52317481540899502</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.96768343675815105</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.77322514244920704</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.89366593371766301</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.82451498251563604</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.93141602657934897</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.74302350456626798</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.54403841763934402</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.96685129432783801</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.75426477504384104</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.99265924141897499</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.57377978767853199</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.90489652270140797</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.94718558089696803</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.95746952815070097</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.98528515173876197</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.57443040748032603</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.50501747538437503</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.74330960164356596</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.90128833956883403</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.58027721412987099</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.86418455998036303</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.84652134445828497</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.53137634041209103</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.75984103386068602</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.52084128851929601</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.82785590604235904</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.80669887111788396</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.94718558089696803</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.75545589076410502</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.57045302636064898</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.74412236459597603</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.993861222875837</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.75318948874039404</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.97853873488160703</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.56129931559518698</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.52001208807376398</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.80291033628995401</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.87784904215285298</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.53294550278660602</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.83019520960681703</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.96781213940121202</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.84854642427637295</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.52091944970511395</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.98143653908655804</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.84155055914140697</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.86563071919316903</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.74312582015880302</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.74357756760104399</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.505124432203229</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.77103809191446204</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.52208451146150403</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.85654363174523596</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.96681158180747695</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.98650386939046997</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.75114215130840101</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.85143872001762699</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.53733983147650999</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.513238468895725</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.94179530111030596</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.50517521512449004</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>0.94718558089696803</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>0.57554623646581304</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0.53959584627359403</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.54403841763934402</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0.74360651330900396</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.74627981514814101</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>0.78987092992202201</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>0.80999174087330506</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.99315256074381397</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>0.51744829591265296</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>0.889135144522325</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>0.97982708350866199</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>0.92442142317581599</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>0.53959584627359403</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>0.74621754461910506</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>0.77148618734153396</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>0.52145658632805503</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>0.62650612160519104</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>0.52232939444234305</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.95092669860238099</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>0.82373068287547302</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>0.88960898915594</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>0.914092501506786</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.53066888063635997</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>0.95782772603422595</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>0.50517578379855999</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>0.53733983147650999</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>0.53294550278660602</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>0.84852833094496605</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>0.74380732940875804</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>0.79479596507957295</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>0.88333994827255402</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>0.53294550278660602</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>0.52601766459514998</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>0.94718558089696803</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>0.89285280248372001</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>0.96281792305166003</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>0.74302860478138799</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>0.98528515173876197</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>0.53294550278660602</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>0.53959584627359403</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>0.81221160518692903</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>0.99761952083513505</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>0.82767468802298305</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>0.76143230731665601</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>0.885106661226157</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>0.89493154237446004</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>0.51153191402197695</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>0.53837502977607798</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>0.51168469394258498</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>0.96430671333579299</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>0.74410953185953499</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>0.82017101225930999</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>0.80881271958794598</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>0.97864524875989301</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>0.89061082534580704</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>0.99544177457158101</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>0.90175028019917303</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>0.79966784050200301</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>0.52854468812084998</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>0.89318010319977803</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>0.74369298925046801</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>0.96603108124164405</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>0.83508604846318202</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>0.89247909384846202</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>0.97638498546910402</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>0.74564630731308301</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>0.77599135952325404</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>0.91925875979941396</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>0.80011795410952902</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>0.53294550278660602</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>0.53316714710443702</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>0.99726827332550405</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>0.81278548758654401</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>0.52091944970511395</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>0.52854468812084998</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>0.52718519274847997</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>0.51074267246284399</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>0.74310260343731205</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>0.506767289645359</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>0.81140139439930403</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>0.94780428382191095</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>0.99408633334983498</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>0.53959584627359403</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>0.79480664811063795</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>0.76091500715230598</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>0.94365332927998302</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>0.83203094091510299</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>0.52854468812084998</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>0.509232851659562</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>0.50471655653082503</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>0.51605744753767502</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>0.74380732940875804</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>0.50426679286410103</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>0.97546897548295197</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>0.97362985292538295</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>0.53733983147650999</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>0.51744829591265296</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>0.79348664472123498</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>0.513238468895725</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>0.52091944970511395</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>0.85685357980518795</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>0.51074267246284399</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>0.77504042176241505</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>0.50788019988436395</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>0.53733983147650999</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>0.98637273809096504</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>0.52091944970511395</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>0.85654363174523596</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>0.97228240487498396</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>0.95890154978593001</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>0.85901124056406497</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>0.56490615608199701</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>0.53231463333601503</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>0.93036528032694399</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>0.82150058812362003</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>0.81595017532485403</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>0.55970985879186097</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>0.50888977348821796</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>0.96044202959941105</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>0.508833645488734</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>0.99736455906337795</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>0.83610813363033898</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>0.85753179961327697</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>0.90304734465954395</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>0.68906425396313098</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>0.99523601351705004</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>0.94718558089696803</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>0.74390597352037402</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>0.85932960529656499</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>0.98528515173876197</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>0.74628215404282805</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>0.82258537997203396</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>0.86436502817752103</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>0.94517769375815996</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>0.74391291645366597</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>0.50424903204277904</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>0.96593147482656505</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>0.82767468802298305</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>0.972978160507046</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>0.89331176099700105</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>0.52145658632805503</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>0.81221160518692903</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>0.50347399965435902</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>0.54403841763934402</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>0.53959584627359403</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>0.74299076238613804</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>0.94812683807242504</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>0.51860150758355805</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>0.97405398998387305</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>0.91241445243913</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>0.52182996414682903</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>0.78641892096105304</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>0.81914120397996204</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>0.61850811645424597</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>0.52502942660894802</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>0.520976799666789</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>0.97487112657677</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>0.899915381251568</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>0.83511651869796799</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>0.95340966881873701</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>0.96555364754139705</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>0.88103154610642898</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>0.74284284554998403</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>0.53733983147650999</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>0.52091944970511395</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>0.89331176099700105</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>0.79377054775167</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>0.87418973683268697</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>0.99073342962545297</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>0.51969918930061798</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>0.54836994861931698</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>0.525031078863062</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>0.84479904047080501</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>0.95782772603422595</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>0.94310724559084802</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>0.52649336784119705</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>0.90269955141647196</c:v>
-                </c:pt>
-                <c:pt idx="387">
-                  <c:v>0.51160735394850698</c:v>
-                </c:pt>
-                <c:pt idx="388">
-                  <c:v>0.94291298183102501</c:v>
-                </c:pt>
-                <c:pt idx="389">
-                  <c:v>0.92835871849453</c:v>
-                </c:pt>
-                <c:pt idx="390">
-                  <c:v>0.51943948448842103</c:v>
-                </c:pt>
-                <c:pt idx="391">
-                  <c:v>0.99208583836665498</c:v>
-                </c:pt>
-                <c:pt idx="392">
-                  <c:v>0.74300870379111505</c:v>
-                </c:pt>
-                <c:pt idx="393">
-                  <c:v>0.94608904027734897</c:v>
-                </c:pt>
-                <c:pt idx="394">
-                  <c:v>0.50558349833331095</c:v>
-                </c:pt>
-                <c:pt idx="395">
-                  <c:v>0.78331802213797397</c:v>
-                </c:pt>
-                <c:pt idx="396">
-                  <c:v>0.95746952815070097</c:v>
-                </c:pt>
-                <c:pt idx="397">
-                  <c:v>0.99736455906337795</c:v>
-                </c:pt>
-                <c:pt idx="398">
-                  <c:v>0.86563071919316903</c:v>
-                </c:pt>
-                <c:pt idx="399">
-                  <c:v>0.76181798716009197</c:v>
-                </c:pt>
-                <c:pt idx="400">
-                  <c:v>0.69711730411342798</c:v>
-                </c:pt>
-                <c:pt idx="401">
-                  <c:v>0.56312423020925595</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="59466496"/>
-        <c:axId val="59898880"/>
+        <c:axId val="72588672"/>
+        <c:axId val="72599040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59466496"/>
+        <c:axId val="72588672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0001"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="1400"/>
+                  <a:t>Entropy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -4954,18 +2510,37 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59898880"/>
+        <c:crossAx val="72599040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59898880"/>
+        <c:axId val="72599040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.05"/>
           <c:min val="0.4"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="1400"/>
+                  <a:t>SSIM</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -4978,30 +2553,16 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59466496"/>
+        <c:crossAx val="72588672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" baseline="0"/>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5012,15 +2573,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5329,8 +2890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>